<commit_message>
update Fei out 11.5
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -436,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+      <selection activeCell="E24" sqref="B24:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -843,6 +843,23 @@
       </c>
       <c r="E23" s="6">
         <v>751000000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="3">
+        <v>44549</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="4">
+        <v>-11500000</v>
+      </c>
+      <c r="E24" s="6">
+        <v>783500000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>